<commit_message>
Final analysis updates before CSEDM submission
</commit_message>
<xml_diff>
--- a/performance_graphs.xlsx
+++ b/performance_graphs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t xml:space="preserve">MAE</t>
   </si>
@@ -31,16 +31,28 @@
     <t xml:space="preserve">Mean Grade</t>
   </si>
   <si>
+    <t xml:space="preserve">TF-IDF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Code2Vec</t>
   </si>
   <si>
-    <t xml:space="preserve">DeepWalk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Node2Vec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TF-IDF</t>
+    <t xml:space="preserve">NC-DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC-N2V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC-DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC-N2V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC-DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC-N2V</t>
   </si>
   <si>
     <t xml:space="preserve">Linear Regression</t>
@@ -281,7 +293,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -310,14 +322,14 @@
             <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -338,6 +350,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -348,13 +365,13 @@
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -366,16 +383,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.185391</c:v>
+                  <c:v>0.18836014957265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.163058</c:v>
+                  <c:v>0.177351859460424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15004</c:v>
+                  <c:v>0.156263760544262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.149417</c:v>
+                  <c:v>0.150005179590072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,14 +416,14 @@
             <a:solidFill>
               <a:srgbClr val="ed7d31"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -427,6 +444,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -437,13 +459,13 @@
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -455,16 +477,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.185391</c:v>
+                  <c:v>0.18836014957265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.163058</c:v>
+                  <c:v>0.177351864773676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15004</c:v>
+                  <c:v>0.163143584084327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.149417</c:v>
+                  <c:v>0.150005179635865</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -488,14 +510,14 @@
             <a:solidFill>
               <a:srgbClr val="a5a5a5"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -516,6 +538,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -526,13 +553,13 @@
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -544,16 +571,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.185391</c:v>
+                  <c:v>0.18836014957265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.168861</c:v>
+                  <c:v>0.181343749206415</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.143486</c:v>
+                  <c:v>0.153870881645674</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.151841</c:v>
+                  <c:v>0.16009502192846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -577,14 +604,14 @@
             <a:solidFill>
               <a:srgbClr val="ffc000"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -605,6 +632,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -615,13 +647,13 @@
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -633,16 +665,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.185391</c:v>
+                  <c:v>0.18836014957265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.159114</c:v>
+                  <c:v>0.177351864773676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.150031</c:v>
+                  <c:v>0.163143581874525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.149651</c:v>
+                  <c:v>0.150005179635864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,17 +682,17 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="77469323"/>
-        <c:axId val="23399500"/>
+        <c:axId val="28201396"/>
+        <c:axId val="98727139"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77469323"/>
+        <c:axId val="28201396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -686,7 +718,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23399500"/>
+        <c:crossAx val="98727139"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -694,7 +726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23399500"/>
+        <c:axId val="98727139"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,13 +765,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77469323"/>
+        <c:crossAx val="28201396"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -749,7 +781,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -819,7 +851,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -848,14 +880,14 @@
             <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -876,44 +908,79 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:f>Sheet1!$B$18:$J$18</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FC-DW</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PC-DW</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PC-N2V</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$E$19</c:f>
+              <c:f>Sheet1!$B$19:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.229133991655797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.209201</c:v>
+                  <c:v>0.177351859460424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.194178</c:v>
+                  <c:v>0.156263760544262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.193812</c:v>
+                  <c:v>0.150005179590072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.149966232741678</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.143467722346929</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.142702464174339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14489639193688</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.142610436280459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,14 +1004,14 @@
             <a:solidFill>
               <a:srgbClr val="ed7d31"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -965,44 +1032,79 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:f>Sheet1!$B$18:$J$18</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FC-DW</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PC-DW</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PC-N2V</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$E$20</c:f>
+              <c:f>Sheet1!$B$20:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.229133991655797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.209201</c:v>
+                  <c:v>0.177351864773676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.194178</c:v>
+                  <c:v>0.163143584084327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.193812</c:v>
+                  <c:v>0.150005179635865</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.149966232913944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.145986373017538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.142702767383279</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.144896376871924</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14260897114147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,14 +1128,14 @@
             <a:solidFill>
               <a:srgbClr val="a5a5a5"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1054,44 +1156,79 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:f>Sheet1!$B$18:$J$18</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FC-DW</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PC-DW</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PC-N2V</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$E$21</c:f>
+              <c:f>Sheet1!$B$21:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.229133991655797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.214294</c:v>
+                  <c:v>0.181343749206415</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18859</c:v>
+                  <c:v>0.153870881645674</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.195351</c:v>
+                  <c:v>0.16009502192846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15643403072368</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.144398430906168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.143449531081621</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.142531405823383</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.143872517531968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1115,14 +1252,14 @@
             <a:solidFill>
               <a:srgbClr val="ffc000"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1143,44 +1280,79 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:f>Sheet1!$B$18:$J$18</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Mean Grade</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Code2Vec</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>DeepWalk</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Node2Vec</c:v>
+                  <c:v>NC-DW</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FC-DW</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FC-N2V</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PC-DW</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PC-N2V</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$22:$E$22</c:f>
+              <c:f>Sheet1!$B$22:$J$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.229133991655797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.205285</c:v>
+                  <c:v>0.177351864773676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.194052</c:v>
+                  <c:v>0.163143581874525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.193925</c:v>
+                  <c:v>0.150005179635864</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.149966232913946</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.145986363601583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.142702767397631</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.144896376872371</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.142608971041476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1188,17 +1360,17 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="49024074"/>
-        <c:axId val="31578551"/>
+        <c:axId val="1137087"/>
+        <c:axId val="21824361"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49024074"/>
+        <c:axId val="1137087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1224,7 +1396,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31578551"/>
+        <c:crossAx val="21824361"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1232,7 +1404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31578551"/>
+        <c:axId val="21824361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,13 +1443,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49024074"/>
+        <c:crossAx val="1137087"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1287,7 +1459,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1334,9 +1506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>381600</xdr:colOff>
+      <xdr:colOff>381240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1344,8 +1516,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7544160" y="0"/>
-        <a:ext cx="4589280" cy="2742840"/>
+        <a:off x="9495000" y="0"/>
+        <a:ext cx="5713560" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1357,16 +1529,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>931680</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>165600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>437760</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>415440</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1374,8 +1546,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7599960" y="2969640"/>
-        <a:ext cx="4589640" cy="2742840"/>
+        <a:off x="3135240" y="4371840"/>
+        <a:ext cx="5925240" cy="2872800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1393,17 +1565,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.11"/>
   </cols>
   <sheetData>
@@ -1431,90 +1603,150 @@
       <c r="F2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.185391</v>
+        <v>0.18836014957265</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.163058</v>
+        <v>0.177351859460424</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.15004</v>
+        <v>0.156263760544262</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0.149417</v>
+        <v>0.150005179590072</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.180945</v>
+        <v>0.149966232741678</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.143467722346929</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.142702464174339</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.14489639193688</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.142610436280459</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.185391</v>
+        <v>0.18836014957265</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.163058</v>
+        <v>0.177351864773676</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.15004</v>
+        <v>0.163143584084327</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.149417</v>
+        <v>0.150005179635865</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.180945</v>
+        <v>0.149966232913944</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.145986373017538</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.142702767383279</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.144896376871924</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.14260897114147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.185391</v>
+        <v>0.18836014957265</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.168861</v>
+        <v>0.181343749206415</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.143486</v>
+        <v>0.153870881645674</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.151841</v>
+        <v>0.16009502192846</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.168473</v>
+        <v>0.15643403072368</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.144398430906168</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.143449531081621</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.142531405823383</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.143872517531968</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.185391</v>
+        <v>0.18836014957265</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.159114</v>
+        <v>0.177351864773676</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.150031</v>
+        <v>0.163143581874525</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.149651</v>
+        <v>0.150005179635864</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.180945</v>
+        <v>0.149966232913946</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.145986363601583</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.142702767397631</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.144896376872371</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.142608971041476</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,99 +1768,159 @@
       <c r="F18" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="G18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.229133991655797</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.209201</v>
+        <v>0.177351859460424</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.194178</v>
+        <v>0.156263760544262</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0.193812</v>
+        <v>0.150005179590072</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.221827</v>
+        <v>0.149966232741678</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0.143467722346929</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.142702464174339</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0.14489639193688</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.142610436280459</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.229133991655797</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.209201</v>
+        <v>0.177351864773676</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.194178</v>
+        <v>0.163143584084327</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>0.193812</v>
+        <v>0.150005179635865</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.221827</v>
+        <v>0.149966232913944</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0.145986373017538</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.142702767383279</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0.144896376871924</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.14260897114147</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.229133991655797</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0.214294</v>
+        <v>0.181343749206415</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.18859</v>
+        <v>0.153870881645674</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>0.195351</v>
+        <v>0.16009502192846</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0.206396</v>
+        <v>0.15643403072368</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0.144398430906168</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.143449531081621</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0.142531405823383</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0.143872517531968</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.229133991655797</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0.205285</v>
+        <v>0.177351864773676</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.194052</v>
+        <v>0.163143581874525</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>0.193925</v>
+        <v>0.150005179635864</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.221827</v>
+        <v>0.149966232913946</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0.145986363601583</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.142702767397631</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0.144896376872371</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0.142608971041476</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,10 +1928,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,10 +1939,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,10 +1950,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,10 +1961,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,10 +1972,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,10 +1983,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,10 +1994,10 @@
         <v>6</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,10 +2005,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,10 +2016,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,10 +2027,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,10 +2038,10 @@
         <v>10</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,10 +2049,10 @@
         <v>11</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,10 +2060,10 @@
         <v>12</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,10 +2071,10 @@
         <v>13</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,10 +2082,10 @@
         <v>14</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,10 +2093,10 @@
         <v>15</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,16 +2104,16 @@
         <v>16</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>